<commit_message>
change output format to elemenLines instead of eChannels
</commit_message>
<xml_diff>
--- a/2D_FL_microscopy/absorption_length_table.xlsx
+++ b/2D_FL_microscopy/absorption_length_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panpanhuang/GitHub/FL_tomography/2D_FL_microscopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DD13B8-D861-FA44-99ED-A4F809A71C33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7C4406-3864-2B45-AA0B-27DD4D633896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="460" windowWidth="24460" windowHeight="14240" xr2:uid="{EB7C6BB4-8D5B-2349-B5D6-7FBABF1507EC}"/>
+    <workbookView xWindow="15240" yWindow="520" windowWidth="24460" windowHeight="14240" xr2:uid="{EB7C6BB4-8D5B-2349-B5D6-7FBABF1507EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="18">
   <si>
     <t>C</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>linear absorption coefficient (1/um)</t>
+  </si>
+  <si>
+    <t>absorption length (um)</t>
   </si>
 </sst>
 </file>
@@ -119,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D024EAD-C9CA-444A-A951-A77D5F56A9A1}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -889,9 +893,521 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
+    <row r="20" spans="1:9">
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>277</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <f>1/E3</f>
+        <v>3.7864445285876562</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" ref="F22:I22" si="0">1/F3</f>
+        <v>1.6518004625041294</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.30605374303727734</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5169902912621358</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.78690588605602774</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>524.9</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" ref="E23:I23" si="1">1/E4</f>
+        <v>0.83808246731478375</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="1"/>
+        <v>7.7339520494972929</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3246787653993906</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>0.47089847428894327</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>2.6116479498563594</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>1739.2</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" ref="E24:I24" si="2">1/E5</f>
+        <v>21.929824561403507</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="2"/>
+        <v>9.7181729834791053</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>27.855153203342617</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="2"/>
+        <v>8.6355785837651116</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="2"/>
+        <v>4.2973785990545768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>1739.8</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" ref="E25:I25" si="3">1/E6</f>
+        <v>21.978021978021978</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="3"/>
+        <v>9.7276264591439681</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="3"/>
+        <v>27.855153203342617</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="3"/>
+        <v>8.6430423509075194</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="3"/>
+        <v>4.301075268817204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>1837</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" ref="E26:I26" si="4">1/E7</f>
+        <v>25.706940874035993</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="4"/>
+        <v>11.325028312570781</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="4"/>
+        <v>32.258064516129032</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="4"/>
+        <v>9.9800399201596814</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="4"/>
+        <v>4.9431537320810675</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>3688.8</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27:I27" si="5">1/E8</f>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="5"/>
+        <v>84.745762711864415</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="5"/>
+        <v>17.793594306049823</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="5"/>
+        <v>65.78947368421052</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="5"/>
+        <v>31.347962382445143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>3692.3</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" ref="E28:I28" si="6">1/E9</f>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="6"/>
+        <v>84.745762711864415</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="6"/>
+        <v>17.857142857142858</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="6"/>
+        <v>65.78947368421052</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="6"/>
+        <v>31.446540880503143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>4013.1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" ref="E29:I29" si="7">1/E10</f>
+        <v>270.27027027027026</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="7"/>
+        <v>108.69565217391305</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="7"/>
+        <v>22.271714922048996</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="7"/>
+        <v>82.644628099173559</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="7"/>
+        <v>39.370078740157481</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>6392.1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" ref="E30:I30" si="8">1/E11</f>
+        <v>31.746031746031747</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="8"/>
+        <v>434.78260869565219</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="8"/>
+        <v>81.300813008130078</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="8"/>
+        <v>31.746031746031747</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="8"/>
+        <v>140.8450704225352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>6405.2</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" ref="E31:I31" si="9">1/E12</f>
+        <v>1111.1111111111111</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="9"/>
+        <v>434.78260869565219</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="9"/>
+        <v>81.967213114754088</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="9"/>
+        <v>31.847133757961785</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="9"/>
+        <v>140.8450704225352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>7059.3</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" ref="E32:I32" si="10">1/E13</f>
+        <v>1428.5714285714287</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="10"/>
+        <v>588.23529411764707</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="10"/>
+        <v>107.52688172043011</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="10"/>
+        <v>41.32231404958678</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="10"/>
+        <v>185.18518518518516</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>717.9</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" ref="E33:I33" si="11">1/E14</f>
+        <v>1.8789928598271326</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="11"/>
+        <v>0.97172286463900504</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="11"/>
+        <v>2.8760425654299682</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="11"/>
+        <v>0.95520106982519826</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="11"/>
+        <v>1.3170025023047545</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>704.8</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" ref="E34:I34" si="12">1/E15</f>
+        <v>1.7873100983020553</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="12"/>
+        <v>0.92954080684142026</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="12"/>
+        <v>2.74423710208562</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="12"/>
+        <v>0.91374269005847952</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="12"/>
+        <v>4.5641259698767689</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>20000</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" ref="E35:I35" si="13">1/E16</f>
+        <v>22624.434389140271</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="13"/>
+        <v>11556.551987149114</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="13"/>
+        <v>2500</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="13"/>
+        <v>769.23076923076928</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="13"/>
+        <v>384.61538461538464</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E20:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>